<commit_message>
Excel de event storming para los 3 contextos IMPORTANTE: Aún no tienen la descripción adecuada, para que lo tengan en cuenta
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 7/Reservas - Event Storming.xlsx
+++ b/Doo-Doc/Seccion # 7/Reservas - Event Storming.xlsx
@@ -5,21 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Seccion # 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC67C3-1186-4598-8439-4D5DD2666137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{27DC67C3-1186-4598-8439-4D5DD2666137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F832E2F3-6657-42DD-ADEE-3CAE6422646E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
     <sheet name="Listado Objetos de Dominio" sheetId="67" r:id="rId2"/>
-    <sheet name="Ciudad" sheetId="66" r:id="rId3"/>
-    <sheet name="Corregimiento" sheetId="24" r:id="rId4"/>
-    <sheet name="Departamento" sheetId="68" r:id="rId5"/>
-    <sheet name="Paìs" sheetId="69" r:id="rId6"/>
+    <sheet name="ZonaComun" sheetId="66" r:id="rId3"/>
+    <sheet name="Turno" sheetId="24" r:id="rId4"/>
+    <sheet name="Residente" sheetId="68" r:id="rId5"/>
+    <sheet name="Reserva" sheetId="69" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Listado Objetos de Dominio'!$A$3:$B$6</definedName>
   </definedNames>
@@ -49,7 +54,7 @@
     <author>WIDER FARID SANCHEZ GARZON</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{3EAB824B-761A-446E-8B9A-62511A69DCED}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{D186447A-5023-4682-B892-AD2B269570CB}">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>Descripción</t>
   </si>
@@ -174,40 +179,118 @@
     <t>Descripción contexto</t>
   </si>
   <si>
-    <t>Delimitaciones</t>
-  </si>
-  <si>
     <t>Contexto cuya motivación es ofrecer las ubicaciones geogràficas de Pais, Departamento, Ciudad y Corregimiento.</t>
   </si>
   <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Corregimiento</t>
-  </si>
-  <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>Paìs</t>
-  </si>
-  <si>
     <t>Objeto de dominio que representa a cada uno de los países donde pueden estar ubicadas las sedes de las Universidad Católica de Oriente y en las cuales se pueden realizar apuestas.</t>
   </si>
   <si>
     <t>Objeto de dominio que representa a cada uno de los departamentos asociados a los países donde pueden estar ubicadas las sedes de las Universidad Católica de Oriente y en las cuales se pueden realizar apuestas.</t>
   </si>
   <si>
-    <t>Países buscados</t>
-  </si>
-  <si>
-    <t>País registrado</t>
-  </si>
-  <si>
-    <t>País dado de baja</t>
-  </si>
-  <si>
-    <t>Estado país modificado</t>
+    <t>Reservas</t>
+  </si>
+  <si>
+    <t>ZonaComun</t>
+  </si>
+  <si>
+    <t>Referenciado</t>
+  </si>
+  <si>
+    <t>Conjuntos Residenciales</t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>Residente</t>
+  </si>
+  <si>
+    <t>Residentes</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>Zona común creada</t>
+  </si>
+  <si>
+    <t>nombre zona común modificado</t>
+  </si>
+  <si>
+    <t>Imagen zona común modificado</t>
+  </si>
+  <si>
+    <t>Descripción zona común modificado</t>
+  </si>
+  <si>
+    <t>Capacidad zona común modificado</t>
+  </si>
+  <si>
+    <t>hora de apertura zona común modificado</t>
+  </si>
+  <si>
+    <t>Hora de cierre zona común modificado</t>
+  </si>
+  <si>
+    <t>ID conjunto residencial asociado</t>
+  </si>
+  <si>
+    <t>Zona común deshabilitada</t>
+  </si>
+  <si>
+    <t>Zona común eliminada</t>
+  </si>
+  <si>
+    <t>Turno creado</t>
+  </si>
+  <si>
+    <t>Turno buscado</t>
+  </si>
+  <si>
+    <t>número de turno turno modificado</t>
+  </si>
+  <si>
+    <t>Hora de inicio turno modificada</t>
+  </si>
+  <si>
+    <t>Hora de finalización turno modificada</t>
+  </si>
+  <si>
+    <t>Turno eliminado</t>
+  </si>
+  <si>
+    <t>Residente Buscado</t>
+  </si>
+  <si>
+    <t>Residente admitido</t>
+  </si>
+  <si>
+    <t>Nombre y Apellido residente modificado</t>
+  </si>
+  <si>
+    <t>Correo electronico modificado</t>
+  </si>
+  <si>
+    <t>Número de contacto modificado</t>
+  </si>
+  <si>
+    <t>Puede reservar Residente modificado</t>
+  </si>
+  <si>
+    <t>Reserva creada</t>
+  </si>
+  <si>
+    <t>Reserva buscada</t>
+  </si>
+  <si>
+    <t>Turno Conjunto residencial modificado</t>
+  </si>
+  <si>
+    <t>Estado Reserva modificado</t>
+  </si>
+  <si>
+    <t>Reserva cancelada</t>
   </si>
 </sst>
 </file>
@@ -371,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -503,21 +586,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -532,6 +600,167 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -546,7 +775,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -588,116 +817,206 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,22 +1062,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>493059</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>354106</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>20171</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>708660</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CB29462-D31B-A6EE-3581-83C2F67CB6C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED49814A-5E19-41B4-BF26-6B6C70CAC698}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -781,8 +1100,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="493059" y="67236"/>
-          <a:ext cx="7055223" cy="3314700"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9386495" cy="5611458"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -802,6 +1121,104 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="ZonaComun"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Agenda"/>
+      <sheetName val="Publicación"/>
+      <sheetName val="Turno"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>ConjuntoResidencial</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>ZonaComun</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="ZonaComun"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Agenda"/>
+      <sheetName val="Publicacion"/>
+      <sheetName val="Turno"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Descripción en términos del negocio del objeto de dominio 2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Residente"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1104,18 +1521,18 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18"/>
     </row>
   </sheetData>
@@ -1129,108 +1546,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02388B9D-0652-49D5-BF62-A59B793D6DFC}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="32"/>
     </row>
-    <row r="2" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="C6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1239,10 +1656,10 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A4" location="Ciudad!A1" display="Ciudad" xr:uid="{78FD4B04-C4A6-4442-9F4A-8F86F773C6D4}"/>
-    <hyperlink ref="A5" location="Corregimiento!A1" display="Corregimiento" xr:uid="{02C9F19B-EE12-42DD-8827-5C5B317B717F}"/>
-    <hyperlink ref="A6" location="Departamento!A1" display="Departamento" xr:uid="{7E61E3F0-0C27-49BA-8A71-784A949CFF1B}"/>
-    <hyperlink ref="A7" location="Paìs!A1" display="Paìs" xr:uid="{16A5D6ED-9AB1-4C42-A079-55252FFDC832}"/>
+    <hyperlink ref="A4" location="Ciudad!A1" display="Ciudad" xr:uid="{9D332338-D074-42C3-B71A-AC00EB1DEE2D}"/>
+    <hyperlink ref="A5" location="Corregimiento!A1" display="Corregimiento" xr:uid="{5DE8806E-3B50-4D64-8FCB-B505612BF7AC}"/>
+    <hyperlink ref="A6" location="Departamento!A1" display="Departamento" xr:uid="{26AA4430-F2BA-40AA-8E27-B767044D9379}"/>
+    <hyperlink ref="A7" location="Paìs!A1" display="Paìs" xr:uid="{0ABDB78F-3DEA-44D4-B937-E86E7AE94CB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1252,173 +1669,173 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D4" sqref="D1:D1048576"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48" t="str">
-        <f>'Listado Objetos de Dominio'!$A$4</f>
-        <v>Ciudad</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
+      <c r="B2" s="62" t="str">
+        <f>'[1]Listado Objetos de Dominio'!A5</f>
+        <v>ZonaComun</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50" t="str">
-        <f>'Listado Objetos de Dominio'!$B$4</f>
-        <v>Descripción en términos del negocio del objeto de dominio 1</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="B3" s="65" t="str">
+        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
+        <v>Descripción en términos del negocio del objeto de dominio 2</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="67"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="59" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="41" t="s">
+      <c r="F5" s="38"/>
+      <c r="G5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="44" t="s">
+      <c r="H5" s="47"/>
+      <c r="I5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="19" t="s">
+      <c r="L5" s="57"/>
+      <c r="M5" s="60"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1427,13 +1844,13 @@
       <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="53"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1443,12 +1860,14 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1458,12 +1877,14 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1473,28 +1894,136 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="18"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="D5:D6"/>
@@ -1510,12 +2039,11 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{F92E8141-0BAA-4CFF-A2AA-790349ADA214}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{BAD90D86-7311-49B0-A802-02D69BE204D5}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{37F7A469-2AC0-4CB1-B156-30D893D383C8}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{D7459321-069F-47BA-AE26-CDE3CC6623F6}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9AA1B6A8-6EA8-461D-AA5C-B30270EFA5B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1524,174 +2052,174 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48" t="str">
-        <f>'Listado Objetos de Dominio'!$A$5</f>
-        <v>Corregimiento</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
+      <c r="B2" s="69" t="str">
+        <f>'Listado Objetos de Dominio'!A5</f>
+        <v>Turno</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50" t="str">
-        <f>'Listado Objetos de Dominio'!$B$5</f>
+      <c r="B3" s="71" t="str">
+        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
         <v>Descripción en términos del negocio del objeto de dominio 2</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="76" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="41" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="44" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="19" t="s">
+      <c r="L5" s="75"/>
+      <c r="M5" s="76"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="81"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1700,13 +2228,13 @@
       <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="79"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="76"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1716,12 +2244,14 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1731,12 +2261,14 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1746,28 +2278,68 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="18"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -1783,13 +2355,11 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{79C12EC1-52AC-413E-AC64-706EBBEE7DDD}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{CEFBA896-B5C8-4F54-8445-F270CCC4F878}"/>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{F84D1E52-B8E1-4C63-BC9C-5D02F82CEE8F}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{3C600C01-7AD0-4985-B5B8-FCEC95433F28}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{98FFE329-8AA7-4A22-8E93-909E4C34D819}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{232AD333-CFCE-4ACF-9E76-9BD38850152F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1797,188 +2367,188 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48" t="str">
-        <f>'Listado Objetos de Dominio'!$A$6</f>
-        <v>Departamento</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
+      <c r="B2" s="69" t="str">
+        <f>'Listado Objetos de Dominio'!A6</f>
+        <v>Residente</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50" t="str">
-        <f>'Listado Objetos de Dominio'!$B$6</f>
-        <v>Objeto de dominio que representa a cada uno de los departamentos asociados a los países donde pueden estar ubicadas las sedes de las Universidad Católica de Oriente y en las cuales se pueden realizar apuestas.</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="B3" s="71" t="str">
+        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
+        <v>Descripción en términos del negocio del objeto de dominio 2</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="L4" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="53" t="s">
+      <c r="M4" s="76" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="41" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="44" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="19" t="s">
+      <c r="L5" s="75"/>
+      <c r="M5" s="76"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="81"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="79"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="76"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1988,12 +2558,14 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -2003,12 +2575,14 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2018,28 +2592,68 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="14" t="s">
+        <v>60</v>
+      </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="18"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="D5:D6"/>
@@ -2055,13 +2669,11 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{D411DE6F-B6AA-4877-8454-AEC23893A3C7}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{53B8BD25-0D2C-4313-BB8B-9056FACF80A3}"/>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{6EF63257-035A-4505-A6A1-EA8BF4D2182C}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9FBAA6B8-5C27-4B0F-828F-C4072A64EB19}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{D0139D04-A27D-4BE9-B834-5429839359DE}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{94142BA0-FFFF-4E30-AC03-536EA62BAABD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2070,173 +2682,173 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8893E27C-63FD-4248-8D03-DE2849BD7525}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48" t="str">
-        <f>'Listado Objetos de Dominio'!$A$7</f>
-        <v>Paìs</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
+      <c r="B2" s="69" t="str">
+        <f>'Listado Objetos de Dominio'!A7</f>
+        <v>Reserva</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50" t="str">
-        <f>'Listado Objetos de Dominio'!$B$7</f>
-        <v>Objeto de dominio que representa a cada uno de los países donde pueden estar ubicadas las sedes de las Universidad Católica de Oriente y en las cuales se pueden realizar apuestas.</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="B3" s="71">
+        <f>'[3]Listado Objetos de Dominio'!$B$7</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="L4" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="53" t="s">
+      <c r="M4" s="83" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="41" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="44" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="19" t="s">
+      <c r="L5" s="82"/>
+      <c r="M5" s="83"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="81"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -2245,13 +2857,13 @@
       <c r="H6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="79"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="83"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2262,13 +2874,13 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -2279,13 +2891,13 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2296,31 +2908,50 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="18"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2336,13 +2967,11 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{7F89A213-BB7C-4D8E-A96A-263D0CDC2BDE}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{21317200-A18A-42CE-A006-FB3497623201}"/>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{A2E0CB1A-981E-4A41-BE15-ACABBB700E6A}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{804E2C57-E5A8-4901-8BC4-4B63A7C4FA3E}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{8EB7698E-1DD1-4373-99C9-673FFA5BD654}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{720BFA19-220B-4457-8396-F7ACF4262B48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2350,21 +2979,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -2508,32 +3122,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
-    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2551,6 +3155,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
+    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6ebbfa72-b3b6-4c1f-8b23-058d4f67f013}" enabled="1" method="Privileged" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
empezando el storming reservas
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 7/Reservas - Event Storming.xlsx
+++ b/Doo-Doc/Seccion # 7/Reservas - Event Storming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9CB297-14CC-48B9-98B6-F86DEB1A267F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F26905-A660-4B6D-BD68-0AC5CD943E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="4" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
   <si>
     <t>Descripción</t>
   </si>
@@ -196,30 +196,6 @@
     <t>Zona común creada</t>
   </si>
   <si>
-    <t>nombre zona común modificado</t>
-  </si>
-  <si>
-    <t>Imagen zona común modificado</t>
-  </si>
-  <si>
-    <t>Descripción zona común modificado</t>
-  </si>
-  <si>
-    <t>Capacidad zona común modificado</t>
-  </si>
-  <si>
-    <t>hora de apertura zona común modificado</t>
-  </si>
-  <si>
-    <t>Hora de cierre zona común modificado</t>
-  </si>
-  <si>
-    <t>ID conjunto residencial asociado</t>
-  </si>
-  <si>
-    <t>Zona común deshabilitada</t>
-  </si>
-  <si>
     <t>Zona común eliminada</t>
   </si>
   <si>
@@ -272,6 +248,75 @@
   </si>
   <si>
     <t>Reserva cancelada</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Crear zona común</t>
+  </si>
+  <si>
+    <t>Acción dónde un administrador podrá crear una zona común</t>
+  </si>
+  <si>
+    <t>información Conjunto residencial</t>
+  </si>
+  <si>
+    <t>Información del conjunto residencial al que se encuentra asociada la zona común que se desea crear.</t>
+  </si>
+  <si>
+    <t>ZonCom-Pol0001</t>
+  </si>
+  <si>
+    <t>No puede existir más de una zona común con el mismo nombre para el mismo conjunto residencial.</t>
+  </si>
+  <si>
+    <t>ZonCom-Pol0002</t>
+  </si>
+  <si>
+    <t>No puede tener un tiempo de uso mayor a la diferencia de hora de cierre y hora de inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar zona común </t>
+  </si>
+  <si>
+    <t>Acción de buscar una zona común especifica</t>
+  </si>
+  <si>
+    <t>Información del conjunto residencial al que se encuentra asociada la zona común que se desea buscar.</t>
+  </si>
+  <si>
+    <t>Zona común buscada</t>
+  </si>
+  <si>
+    <t>Modificar zona común</t>
+  </si>
+  <si>
+    <t>Acción de modificar los atributos de una zona común</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZonaComun </t>
+  </si>
+  <si>
+    <t>Información del conjunto residencial al que se encuentra asociada la zona común que se desea modificar</t>
+  </si>
+  <si>
+    <t>Zona común modificada.</t>
+  </si>
+  <si>
+    <t>Eliminar zona común</t>
+  </si>
+  <si>
+    <t>Acción de eliminar una zona común de un conjunto residencial.</t>
+  </si>
+  <si>
+    <t>Información del conjunto residencial al que se encuentra asociada la zona común que se desea eliminar.</t>
+  </si>
+  <si>
+    <t>ZonCom-Pol0004</t>
+  </si>
+  <si>
+    <t>No puede eliminarse una zona común inexistente.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -750,13 +795,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -843,6 +910,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -855,6 +925,87 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -882,77 +1033,8 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -993,26 +1075,83 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1116,104 +1255,6 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Flujo de eventos en el tiempo"/>
-      <sheetName val="Listado Objetos de Dominio"/>
-      <sheetName val="ConjuntoResidencial"/>
-      <sheetName val="ZonaComun"/>
-      <sheetName val="Administrador"/>
-      <sheetName val="Agenda"/>
-      <sheetName val="Publicación"/>
-      <sheetName val="Turno"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1">
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>ConjuntoResidencial</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>ZonaComun</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Flujo de eventos en el tiempo"/>
-      <sheetName val="Listado Objetos de Dominio"/>
-      <sheetName val="ConjuntoResidencial"/>
-      <sheetName val="ZonaComun"/>
-      <sheetName val="Administrador"/>
-      <sheetName val="Agenda"/>
-      <sheetName val="Publicacion"/>
-      <sheetName val="Turno"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Descripción en términos del negocio del objeto de dominio 2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Flujo de eventos en el tiempo"/>
-      <sheetName val="Listado Objetos de Dominio"/>
-      <sheetName val="ConjuntoResidencial"/>
-      <sheetName val="Administrador"/>
-      <sheetName val="Residente"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -1251,7 +1292,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1295,6 +1336,102 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="ZonaComun"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Agenda"/>
+      <sheetName val="Publicacion"/>
+      <sheetName val="Turno"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Descripción en términos del negocio del objeto de dominio 2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Residente"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos en el tiempo"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="ZonaComun"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="Agenda"/>
+      <sheetName val="Publicacion"/>
+      <sheetName val="Turno"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1643,22 +1780,22 @@
       <c r="A1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="32" t="str">
-        <f>[4]Contextos!$D$14</f>
+      <c r="B2" s="33" t="str">
+        <f>[1]Contextos!$D$14</f>
         <v>Contexto cuya intención enfocarse en la gestión del proceso de reservas de los recursos, incluyendo la disponibilidad de los recursos y las reservas que los residentes realizan.</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -1679,13 +1816,13 @@
         <v>34</v>
       </c>
       <c r="B4" s="26" t="str">
-        <f>'[5]Listado Objetos de Dominio'!$B$3</f>
+        <f>'[2]Listado Objetos de Dominio'!$B$3</f>
         <v>Objeto de dominio que representa a cada una de las reservas creadas por los residente según una zona comun que esta condicionada con una agenda y según la disponibilidad de turno poder reservar el espacio.</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="84" t="str">
+      <c r="D4" s="35" t="str">
         <f>$B$1</f>
         <v>Reservas</v>
       </c>
@@ -1694,40 +1831,40 @@
       <c r="A5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="83" t="str">
-        <f>'[5]Listado Objetos de Dominio'!$B$4</f>
+      <c r="B5" s="30" t="str">
+        <f>'[2]Listado Objetos de Dominio'!$B$4</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="83" t="str">
-        <f>'[5]Listado Objetos de Dominio'!$B$6</f>
+      <c r="B6" s="30" t="str">
+        <f>'[2]Listado Objetos de Dominio'!$B$6</f>
         <v>Objeto de dominio que representa a cada Turno que esta programado con respecto al tiempo de uso según la zona comun y con respecto a la agenda disponible.</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="85"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="26" t="str">
-        <f>'[5]Listado Objetos de Dominio'!$B$5</f>
+        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a un residente que podrá realizar una reserva de una zona común dentro de un conjunto residencial.</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="86"/>
+      <c r="D7" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1749,10 +1886,789 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J13" sqref="J13:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="62" t="str">
+        <f>'[5]Listado Objetos de Dominio'!$B$5</f>
+        <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="68"/>
+      <c r="G4" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="48"/>
+      <c r="I4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="68"/>
+      <c r="G5" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="44"/>
+      <c r="I5" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="54"/>
+      <c r="M5" s="57"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="58"/>
+    </row>
+    <row r="7" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="92"/>
+    </row>
+    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="93"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="98"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="101" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="102"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="105"/>
+    </row>
+    <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+    </row>
+    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="107"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="95"/>
+    </row>
+    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="108" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="108" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="109" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="109" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="108"/>
+      <c r="J13" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="108"/>
+      <c r="L13" s="108"/>
+      <c r="M13" s="108"/>
+    </row>
+    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="108"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="108"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="108"/>
+    </row>
+  </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{9731DD29-410B-49AA-8598-6F81A16BB9B6}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{6D85FC52-830B-4C1A-B3F4-298107124B67}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{81F20DC4-BB3C-4598-A50F-481F0C8E6076}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="73" t="str">
+        <f>'Listado Objetos de Dominio'!A6</f>
+        <v>Turno</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="75" t="str">
+        <f>'[3]Listado Objetos de Dominio'!$B$5</f>
+        <v>Descripción en términos del negocio del objeto de dominio 2</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="77"/>
+      <c r="G4" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="78"/>
+      <c r="I4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="77"/>
+      <c r="G5" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="81"/>
+      <c r="I5" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="79"/>
+      <c r="M5" s="80"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="80"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{3C600C01-7AD0-4985-B5B8-FCEC95433F28}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{98FFE329-8AA7-4A22-8E93-909E4C34D819}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{232AD333-CFCE-4ACF-9E76-9BD38850152F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,84 +2695,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A5</f>
-        <v>ZonaComun</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="B2" s="73" t="str">
+        <f>'Listado Objetos de Dominio'!A7</f>
+        <v>Residente</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34" t="str">
-        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
+      <c r="B3" s="75" t="str">
+        <f>'[3]Listado Objetos de Dominio'!$B$5</f>
         <v>Descripción en términos del negocio del objeto de dominio 2</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="36"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="76"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="52" t="s">
+      <c r="F4" s="77"/>
+      <c r="G4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="78"/>
       <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
@@ -1866,52 +2782,52 @@
       <c r="K4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="61" t="s">
+      <c r="M4" s="80" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="48" t="s">
+      <c r="F5" s="77"/>
+      <c r="G5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="81"/>
+      <c r="I5" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="62"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="80"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="42"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="15" t="s">
         <v>21</v>
       </c>
@@ -1924,11 +2840,11 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="63"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="80"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -1941,7 +2857,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -1958,7 +2874,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -1975,7 +2891,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -1992,7 +2908,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -2009,7 +2925,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -2026,712 +2942,15 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="D5:D6"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{37F7A469-2AC0-4CB1-B156-30D893D383C8}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{D7459321-069F-47BA-AE26-CDE3CC6623F6}"/>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9AA1B6A8-6EA8-461D-AA5C-B30270EFA5B9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
-  <dimension ref="A1:N12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:M3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="68" t="str">
-        <f>'Listado Objetos de Dominio'!A6</f>
-        <v>Turno</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="70" t="str">
-        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
-        <v>Descripción en términos del negocio del objeto de dominio 2</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="76" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="75"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="75"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D5:D6"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{3C600C01-7AD0-4985-B5B8-FCEC95433F28}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{98FFE329-8AA7-4A22-8E93-909E4C34D819}"/>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{232AD333-CFCE-4ACF-9E76-9BD38850152F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
-  <dimension ref="A1:N12"/>
-  <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:M3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="68" t="str">
-        <f>'Listado Objetos de Dominio'!A7</f>
-        <v>Residente</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="70" t="str">
-        <f>'[2]Listado Objetos de Dominio'!$B$5</f>
-        <v>Descripción en términos del negocio del objeto de dominio 2</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="76" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="75"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="75"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="17">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2748,7 +2967,6 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9FBAA6B8-5C27-4B0F-828F-C4072A64EB19}"/>
@@ -2764,7 +2982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8893E27C-63FD-4248-8D03-DE2849BD7525}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -2792,84 +3010,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="68" t="str">
+      <c r="B2" s="73" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Reserva</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="70">
-        <f>'[3]Listado Objetos de Dominio'!$B$7</f>
+      <c r="B3" s="75">
+        <f>'[4]Listado Objetos de Dominio'!$B$7</f>
         <v>0</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="71"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="76"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="67"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73" t="s">
+      <c r="F4" s="77"/>
+      <c r="G4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="78"/>
       <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
@@ -2879,52 +3097,52 @@
       <c r="K4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="81" t="s">
+      <c r="L4" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="82" t="s">
+      <c r="M4" s="86" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="76" t="s">
+      <c r="F5" s="77"/>
+      <c r="G5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="78" t="s">
+      <c r="H5" s="81"/>
+      <c r="I5" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="81"/>
-      <c r="M5" s="82"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="86"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="42"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="15" t="s">
         <v>21</v>
       </c>
@@ -2937,11 +3155,11 @@
       <c r="H6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="82"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="86"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -2954,7 +3172,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -2971,7 +3189,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -2988,7 +3206,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -3005,7 +3223,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
@@ -3022,7 +3240,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -3030,6 +3248,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -3046,7 +3265,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{804E2C57-E5A8-4901-8BC4-4B63A7C4FA3E}"/>
@@ -3059,9 +3277,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3209,27 +3430,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
-    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3253,9 +3462,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
+    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>